<commit_message>
abrir cerrar boveda- ERROR: estado: true, estado: "true", corregir eso
</commit_message>
<xml_diff>
--- a/CurrencyISO.xlsx
+++ b/CurrencyISO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\GitHub\SistCoopEE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
   </bookViews>
@@ -1350,7 +1345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1369,31 +1364,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7590,7 +7570,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7625,7 +7605,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8520,7 +8500,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10642,7 +10622,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10654,11 +10634,12 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.42578125" style="10"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10666,7 +10647,7 @@
       <c r="A1" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>407</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -10677,7 +10658,7 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="9">
         <v>0.1</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -10688,7 +10669,7 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="9">
         <v>0.2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -10699,7 +10680,7 @@
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="9">
         <v>0.3</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -10710,7 +10691,7 @@
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="9">
         <v>0.5</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -10721,7 +10702,7 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -10732,7 +10713,7 @@
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="9">
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -10743,7 +10724,7 @@
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -10754,7 +10735,7 @@
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="9">
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -10765,7 +10746,7 @@
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="9">
         <v>20</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -10776,7 +10757,7 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="9">
         <v>50</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -10787,7 +10768,7 @@
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="9">
         <v>100</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -10798,7 +10779,7 @@
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="9">
         <v>200</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -10809,7 +10790,7 @@
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="9">
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -10820,7 +10801,7 @@
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="9">
         <v>2</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -10831,7 +10812,7 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="9">
         <v>5</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -10842,7 +10823,7 @@
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="9">
         <v>10</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -10853,7 +10834,7 @@
       <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="9">
         <v>20</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -10864,7 +10845,7 @@
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="9">
         <v>50</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -10875,7 +10856,7 @@
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="9">
         <v>100</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -10886,7 +10867,7 @@
       <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="9">
         <v>5</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -10897,7 +10878,7 @@
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="9">
         <v>10</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -10908,7 +10889,7 @@
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="9">
         <v>20</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -10919,7 +10900,7 @@
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="9">
         <v>50</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -10930,7 +10911,7 @@
       <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="9">
         <v>100</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -10941,7 +10922,7 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="9">
         <v>200</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -10952,7 +10933,7 @@
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="9">
         <v>500</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -10961,8 +10942,9 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>